<commit_message>
Fixed x accuracy based on focal length of camera
</commit_message>
<xml_diff>
--- a/tables/feature_localization_testing_results.xlsx
+++ b/tables/feature_localization_testing_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Drill" sheetId="1" r:id="rId1"/>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:T14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S14" sqref="S14:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -569,7 +569,7 @@
       </c>
       <c r="H3">
         <f>ABS(E3-($K$3*1000))</f>
-        <v>14.22300099200001</v>
+        <v>2.2245169633000046</v>
       </c>
       <c r="I3">
         <v>-1.36</v>
@@ -578,8 +578,8 @@
         <v>-0.44</v>
       </c>
       <c r="K3" s="2">
-        <f>0.4-0.203+0.003</f>
-        <v>0.2</v>
+        <f>0.4-0.203+0.003+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
       <c r="O3">
         <f>AVERAGE(F3:F7,F10:F14,F17:F21,F24:F28)</f>
@@ -599,11 +599,11 @@
       </c>
       <c r="S3">
         <f>AVERAGE(H3:H7,H10:H14,H17:H21,H24:H28)</f>
-        <v>13.250680474899998</v>
+        <v>1.4379256874499888</v>
       </c>
       <c r="T3">
         <f>_xlfn.STDEV.P(H3:H7,H10:H14,H17:H21,H24:H28)</f>
-        <v>1.4318473155090097</v>
+        <v>1.2452117860740748</v>
       </c>
     </row>
     <row r="4" spans="2:20">
@@ -629,7 +629,7 @@
       </c>
       <c r="H4">
         <f>ABS(E4-($K$3*1000))</f>
-        <v>14.221592038000011</v>
+        <v>2.223108009300006</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>26</v>
@@ -663,7 +663,7 @@
       </c>
       <c r="H5">
         <f>ABS(E5-($K$3*1000))</f>
-        <v>14.637828039999988</v>
+        <v>2.6393440112999826</v>
       </c>
       <c r="O5" t="s">
         <v>21</v>
@@ -707,7 +707,7 @@
       </c>
       <c r="H6">
         <f>ABS(E6-($K$3*1000))</f>
-        <v>13.923491049999996</v>
+        <v>1.9250070212999901</v>
       </c>
       <c r="O6">
         <f>AVERAGE(F31:F35,F38:F42,F45:F49,F52:F56)</f>
@@ -727,11 +727,11 @@
       </c>
       <c r="S6">
         <f>AVERAGE(H31:H35,H38:H42,H45:H49,H52:H56)</f>
-        <v>13.623883931699975</v>
+        <v>1.8904397705199898</v>
       </c>
       <c r="T6">
         <f>_xlfn.STDEV.P(H31:H35,H38:H42,H45:H49,H52:H561)</f>
-        <v>2.7144691155616107</v>
+        <v>1.5553417988587652</v>
       </c>
     </row>
     <row r="7" spans="2:20">
@@ -757,7 +757,7 @@
       </c>
       <c r="H7">
         <f>ABS(E7-($K$3*1000))</f>
-        <v>13.809608951000001</v>
+        <v>1.8111249222999959</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>24</v>
@@ -837,11 +837,11 @@
       </c>
       <c r="S9">
         <f>AVERAGE(H59:H63,H66:H70,H73:H77,H80:H84)</f>
-        <v>10.78391726189999</v>
+        <v>2.1545246432799927</v>
       </c>
       <c r="T9">
         <f>_xlfn.STDEV.P(H59:H63,H66:H70,H73:H77,H80:H84)</f>
-        <v>2.5499218360051943</v>
+        <v>1.8262796506149472</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -867,7 +867,7 @@
       </c>
       <c r="H10">
         <f>ABS(E10-($K$10*1000))</f>
-        <v>14.767009009999981</v>
+        <v>2.7685249812999757</v>
       </c>
       <c r="I10">
         <v>1.45</v>
@@ -876,8 +876,8 @@
         <v>-0.3</v>
       </c>
       <c r="K10" s="2">
-        <f>0.4-0.205+0.003</f>
-        <v>0.19800000000000004</v>
+        <f>0.4-0.205+0.003+0.0119984840287</f>
+        <v>0.20999848402870003</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>25</v>
@@ -911,7 +911,7 @@
       </c>
       <c r="H11">
         <f>ABS(E11-($K$10*1000))</f>
-        <v>14.808143247999965</v>
+        <v>2.8096592192999594</v>
       </c>
       <c r="O11" t="s">
         <v>21</v>
@@ -955,7 +955,7 @@
       </c>
       <c r="H12">
         <f>ABS(E12-($K$10*1000))</f>
-        <v>15.01644024999996</v>
+        <v>3.0179562212999542</v>
       </c>
       <c r="O12">
         <f>AVERAGE(F87:F91,F94:F98,F101:F105,F108:F112)</f>
@@ -975,11 +975,11 @@
       </c>
       <c r="S12">
         <f>AVERAGE(H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>10.552318041999978</v>
+        <v>2.7089384818500095</v>
       </c>
       <c r="T12">
         <f>_xlfn.STDEV.P(H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>2.4833699644278719</v>
+        <v>0.95925739135161003</v>
       </c>
     </row>
     <row r="13" spans="2:20">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="H13">
         <f>ABS(E13-($K$10*1000))</f>
-        <v>15.043522758999984</v>
+        <v>3.0450387302999786</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>28</v>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="H14">
         <f>ABS(E14-($K$10*1000))</f>
-        <v>15.613490687999985</v>
+        <v>3.6150066592999792</v>
       </c>
       <c r="O14">
         <f>AVERAGE(F3:F7,F10:F14,F17:F21,F24:F28,F31:F35,F38:F42,F45:F49,F52:F56,F59:F63,F66:F70,F73:F77,F80:F84,F87:F91,F94:F98,F101:F105,F108:F112)</f>
@@ -1059,11 +1059,11 @@
       </c>
       <c r="S14">
         <f>AVERAGE(H3:H7,H10:H14,H17:H21,H24:H28,H31:H35,H38:H42,H45:H49,H52:H56,H59:H63,H66:H70,H73:H77,H80:H84,H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>12.052699927624989</v>
+        <v>2.047957145774995</v>
       </c>
       <c r="T14">
         <f>_xlfn.STDEV.P(H3:H7,H10:H14,H17:H21,H24:H28,H31:H35,H38:H42,H45:H49,H52:H56,H59:H63,H66:H70,H73:H77,H80:H84,H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>2.5528786527080141</v>
+        <v>1.5251230469105566</v>
       </c>
     </row>
     <row r="16" spans="2:20">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="H17">
         <f>ABS(E17-($K$17*1000))</f>
-        <v>11.956700282000014</v>
+        <v>4.1783746699991298E-2</v>
       </c>
       <c r="I17">
         <v>-0.51</v>
@@ -1130,8 +1130,8 @@
         <v>2.17</v>
       </c>
       <c r="K17" s="2">
-        <f>0.4-0.203+0.003</f>
-        <v>0.2</v>
+        <f>0.4-0.203+0.003+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H18">
         <f>ABS(E18-($K$17*1000))</f>
-        <v>11.543563709000011</v>
+        <v>0.45492031969999402</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="H19">
         <f>ABS(E19-($K$17*1000))</f>
-        <v>10.951925237000012</v>
+        <v>1.0465587916999937</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="H20">
         <f>ABS(E20-($K$17*1000))</f>
-        <v>11.946875057</v>
+        <v>5.1608971700005668E-2</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="H21">
         <f>ABS(E21-($K$17*1000))</f>
-        <v>11.736063446000003</v>
+        <v>0.26242058270000257</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="H24">
         <f>ABS(E24-($K$24*1000))</f>
-        <v>12.137976460000004</v>
+        <v>0.139492431299999</v>
       </c>
       <c r="I24">
         <v>-0.42</v>
@@ -1302,7 +1302,8 @@
         <v>-1.03</v>
       </c>
       <c r="K24" s="2">
-        <v>0.2</v>
+        <f>0.2+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
     </row>
     <row r="25" spans="2:11">
@@ -1328,7 +1329,7 @@
       </c>
       <c r="H25">
         <f>ABS(E25-($K$24*1000))</f>
-        <v>12.147848170000003</v>
+        <v>0.14936414129999775</v>
       </c>
     </row>
     <row r="26" spans="2:11">
@@ -1354,7 +1355,7 @@
       </c>
       <c r="H26">
         <f>ABS(E26-($K$24*1000))</f>
-        <v>12.147019137000001</v>
+        <v>0.1485351082999955</v>
       </c>
     </row>
     <row r="27" spans="2:11">
@@ -1380,7 +1381,7 @@
       </c>
       <c r="H27">
         <f>ABS(E27-($K$24*1000))</f>
-        <v>12.180311913999986</v>
+        <v>0.18182788529998106</v>
       </c>
     </row>
     <row r="28" spans="2:11">
@@ -1406,7 +1407,7 @@
       </c>
       <c r="H28">
         <f>ABS(E28-($K$24*1000))</f>
-        <v>12.201199059999993</v>
+        <v>0.20271503129998791</v>
       </c>
     </row>
     <row r="30" spans="2:11">
@@ -1464,7 +1465,7 @@
       </c>
       <c r="H31">
         <f>ABS(E31-($K$31*1000))</f>
-        <v>14.549514479999971</v>
+        <v>2.5510304512999653</v>
       </c>
       <c r="I31">
         <v>1.67</v>
@@ -1473,8 +1474,8 @@
         <v>-4.0199999999999996</v>
       </c>
       <c r="K31">
-        <f>0.4-0.208+0.003</f>
-        <v>0.19500000000000003</v>
+        <f>0.4-0.208+0.003+0.0119984840287</f>
+        <v>0.20699848402870002</v>
       </c>
     </row>
     <row r="32" spans="2:11">
@@ -1500,7 +1501,7 @@
       </c>
       <c r="H32">
         <f>ABS(E32-($K$31*1000))</f>
-        <v>13.677309624999964</v>
+        <v>1.6788255962999585</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -1526,7 +1527,7 @@
       </c>
       <c r="H33">
         <f>ABS(E33-($K$31*1000))</f>
-        <v>15.43319617399996</v>
+        <v>3.4347121452999545</v>
       </c>
     </row>
     <row r="34" spans="2:11">
@@ -1552,7 +1553,7 @@
       </c>
       <c r="H34">
         <f>ABS(E34-($K$31*1000))</f>
-        <v>14.576926177999979</v>
+        <v>2.5784421492999741</v>
       </c>
     </row>
     <row r="35" spans="2:11">
@@ -1578,7 +1579,7 @@
       </c>
       <c r="H35">
         <f>ABS(E35-($K$31*1000))</f>
-        <v>15.109108942999967</v>
+        <v>3.1106249142999616</v>
       </c>
     </row>
     <row r="37" spans="2:11">
@@ -1636,7 +1637,7 @@
       </c>
       <c r="H38">
         <f>ABS(E38-($K$38*1000))</f>
-        <v>12.123403537999991</v>
+        <v>0.12491950929998552</v>
       </c>
       <c r="I38">
         <v>-3.77</v>
@@ -1645,8 +1646,8 @@
         <v>-5.22</v>
       </c>
       <c r="K38" s="2">
-        <f>0.4-0.203+0.003</f>
-        <v>0.2</v>
+        <f>0.4-0.203+0.003+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
     </row>
     <row r="39" spans="2:11">
@@ -1672,7 +1673,7 @@
       </c>
       <c r="H39">
         <f>ABS(E39-($K$38*1000))</f>
-        <v>11.968158863000014</v>
+        <v>3.0325165699991885E-2</v>
       </c>
     </row>
     <row r="40" spans="2:11">
@@ -1698,7 +1699,7 @@
       </c>
       <c r="H40">
         <f>ABS(E40-($K$38*1000))</f>
-        <v>12.014329585000013</v>
+        <v>1.5845556300007502E-2</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -1724,7 +1725,7 @@
       </c>
       <c r="H41">
         <f>ABS(E41-($K$38*1000))</f>
-        <v>12.398813268999987</v>
+        <v>0.40032924029998185</v>
       </c>
     </row>
     <row r="42" spans="2:11">
@@ -1750,7 +1751,7 @@
       </c>
       <c r="H42">
         <f>ABS(E42-($K$38*1000))</f>
-        <v>12.783232274999989</v>
+        <v>0.78474824629998352</v>
       </c>
     </row>
     <row r="44" spans="2:11">
@@ -1808,7 +1809,7 @@
       </c>
       <c r="H45">
         <f>ABS(E45-($K$45*1000))</f>
-        <v>16.591949625999973</v>
+        <v>4.5934655972999678</v>
       </c>
       <c r="I45">
         <v>-4.57</v>
@@ -1817,8 +1818,8 @@
         <v>3.44</v>
       </c>
       <c r="K45" s="2">
-        <f>0.4-0.205+0.003</f>
-        <v>0.19800000000000004</v>
+        <f>0.4-0.205+0.003+0.0119984840287</f>
+        <v>0.20999848402870003</v>
       </c>
     </row>
     <row r="46" spans="2:11">
@@ -1844,7 +1845,7 @@
       </c>
       <c r="H46">
         <f>ABS(E46-($K$45*1000))</f>
-        <v>15.501652039999982</v>
+        <v>3.5031680112999766</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -1870,7 +1871,7 @@
       </c>
       <c r="H47">
         <f>ABS(E47-($K$45*1000))</f>
-        <v>16.158531254999986</v>
+        <v>4.1600472262999801</v>
       </c>
     </row>
     <row r="48" spans="2:11">
@@ -1896,7 +1897,7 @@
       </c>
       <c r="H48">
         <f>ABS(E48-($K$45*1000))</f>
-        <v>15.797916715999975</v>
+        <v>3.7994326872999693</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -1922,7 +1923,7 @@
       </c>
       <c r="H49">
         <f>ABS(E49-($K$45*1000))</f>
-        <v>16.42128943299997</v>
+        <v>4.4228054042999645</v>
       </c>
     </row>
     <row r="51" spans="2:11">
@@ -1980,7 +1981,7 @@
       </c>
       <c r="H52">
         <f>ABS(E52-($K$52*1000))</f>
-        <v>11.617709097999978</v>
+        <v>0.38077493070002788</v>
       </c>
       <c r="I52">
         <v>4.7</v>
@@ -1989,8 +1990,8 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="K52" s="2">
-        <f>0.4-0.204+0.003</f>
-        <v>0.19900000000000004</v>
+        <f>0.4-0.204+0.003+0.0119984840287</f>
+        <v>0.21099848402870003</v>
       </c>
     </row>
     <row r="53" spans="2:11">
@@ -2016,7 +2017,7 @@
       </c>
       <c r="H53">
         <f>ABS(E53-($K$52*1000))</f>
-        <v>11.371870636999972</v>
+        <v>0.62661339170003316</v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -2042,7 +2043,7 @@
       </c>
       <c r="H54">
         <f>ABS(E54-($K$52*1000))</f>
-        <v>11.817240845999976</v>
+        <v>0.18124318270002959</v>
       </c>
     </row>
     <row r="55" spans="2:11">
@@ -2068,7 +2069,7 @@
       </c>
       <c r="H55">
         <f>ABS(E55-($K$52*1000))</f>
-        <v>11.382880080999968</v>
+        <v>0.61560394770003768</v>
       </c>
     </row>
     <row r="56" spans="2:11">
@@ -2094,7 +2095,7 @@
       </c>
       <c r="H56">
         <f>ABS(E56-($K$52*1000))</f>
-        <v>11.18264597199996</v>
+        <v>0.81583805670004494</v>
       </c>
     </row>
     <row r="58" spans="2:11">
@@ -2152,7 +2153,7 @@
       </c>
       <c r="H59">
         <f>ABS(E59-($K$59*1000))</f>
-        <v>14.227010110999998</v>
+        <v>2.228526082299993</v>
       </c>
       <c r="I59">
         <v>-0.31</v>
@@ -2161,7 +2162,8 @@
         <v>-9.8699999999999992</v>
       </c>
       <c r="K59" s="2">
-        <v>0.2</v>
+        <f>0.2+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
     </row>
     <row r="60" spans="2:11">
@@ -2187,7 +2189,7 @@
       </c>
       <c r="H60">
         <f t="shared" ref="H60:H63" si="2">ABS(E60-($K$59*1000))</f>
-        <v>13.759658933999987</v>
+        <v>1.7611749052999812</v>
       </c>
     </row>
     <row r="61" spans="2:11">
@@ -2213,7 +2215,7 @@
       </c>
       <c r="H61">
         <f t="shared" si="2"/>
-        <v>14.007085657000005</v>
+        <v>2.0086016282999992</v>
       </c>
     </row>
     <row r="62" spans="2:11">
@@ -2239,7 +2241,7 @@
       </c>
       <c r="H62">
         <f t="shared" si="2"/>
-        <v>13.70402915599999</v>
+        <v>1.7055451272999846</v>
       </c>
     </row>
     <row r="63" spans="2:11">
@@ -2265,7 +2267,7 @@
       </c>
       <c r="H63">
         <f t="shared" si="2"/>
-        <v>13.539637086999988</v>
+        <v>1.5411530582999831</v>
       </c>
     </row>
     <row r="65" spans="2:22">
@@ -2323,7 +2325,7 @@
       </c>
       <c r="H66">
         <f>ABS(E66-($K$66*1000))</f>
-        <v>12.153061991999976</v>
+        <v>0.15457796329997109</v>
       </c>
       <c r="I66">
         <v>2.0099999999999998</v>
@@ -2332,8 +2334,8 @@
         <v>9.83</v>
       </c>
       <c r="K66" s="2">
-        <f>0.4-0.206+0.003</f>
-        <v>0.19700000000000004</v>
+        <f>0.4-0.206+0.003+0.0119984840287</f>
+        <v>0.20899848402870003</v>
       </c>
     </row>
     <row r="67" spans="2:22">
@@ -2359,7 +2361,7 @@
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H70" si="5">ABS(E67-($K$66*1000))</f>
-        <v>11.350557656999968</v>
+        <v>0.64792637170003786</v>
       </c>
     </row>
     <row r="68" spans="2:22">
@@ -2385,7 +2387,7 @@
       </c>
       <c r="H68">
         <f t="shared" si="5"/>
-        <v>11.947526820999968</v>
+        <v>5.0957207700037088E-2</v>
       </c>
     </row>
     <row r="69" spans="2:22">
@@ -2411,7 +2413,7 @@
       </c>
       <c r="H69">
         <f t="shared" si="5"/>
-        <v>11.950659675999958</v>
+        <v>4.7824352700047257E-2</v>
       </c>
     </row>
     <row r="70" spans="2:22">
@@ -2437,7 +2439,7 @@
       </c>
       <c r="H70">
         <f t="shared" si="5"/>
-        <v>11.350335205999983</v>
+        <v>0.64814882270002272</v>
       </c>
     </row>
     <row r="72" spans="2:22">
@@ -2525,7 +2527,7 @@
       </c>
       <c r="H73">
         <f>ABS(E73-($K$73*1000))</f>
-        <v>11.428260305000009</v>
+        <v>0.57022372369996788</v>
       </c>
       <c r="I73">
         <v>-12.88</v>
@@ -2534,7 +2536,8 @@
         <v>11.55</v>
       </c>
       <c r="K73" s="2">
-        <v>0.20399999999999999</v>
+        <f>0.204+0.0119984840287</f>
+        <v>0.21599848402869998</v>
       </c>
       <c r="M73">
         <v>1</v>
@@ -2594,7 +2597,7 @@
       </c>
       <c r="H74">
         <f t="shared" ref="H74:H77" si="8">ABS(E74-($K$73*1000))</f>
-        <v>10.793094491000005</v>
+        <v>1.2053895376999719</v>
       </c>
       <c r="M74">
         <v>2</v>
@@ -2644,7 +2647,7 @@
       </c>
       <c r="H75">
         <f t="shared" si="8"/>
-        <v>10.196409698999986</v>
+        <v>1.802074329699991</v>
       </c>
       <c r="M75">
         <v>3</v>
@@ -2694,7 +2697,7 @@
       </c>
       <c r="H76">
         <f t="shared" si="8"/>
-        <v>9.968322478999994</v>
+        <v>2.030161549699983</v>
       </c>
       <c r="M76">
         <v>4</v>
@@ -2744,7 +2747,7 @@
       </c>
       <c r="H77">
         <f t="shared" si="8"/>
-        <v>10.830645656000002</v>
+        <v>1.1678383726999755</v>
       </c>
       <c r="M77">
         <v>5</v>
@@ -2856,7 +2859,7 @@
       </c>
       <c r="H80">
         <f>ABS(E80-($K$80*1000))</f>
-        <v>6.733206421999995</v>
+        <v>5.265277606699982</v>
       </c>
       <c r="I80">
         <v>9.6300000000000008</v>
@@ -2865,7 +2868,8 @@
         <v>-9.15</v>
       </c>
       <c r="K80" s="2">
-        <v>0.21</v>
+        <f>0.21+0.0119984840287</f>
+        <v>0.22199848402869998</v>
       </c>
       <c r="M80">
         <v>1</v>
@@ -2924,7 +2928,7 @@
       </c>
       <c r="H81">
         <f t="shared" ref="H81:H84" si="11">ABS(E81-($K$80*1000))</f>
-        <v>6.7326861839999879</v>
+        <v>5.2657978446999891</v>
       </c>
       <c r="M81">
         <v>2</v>
@@ -2974,7 +2978,7 @@
       </c>
       <c r="H82">
         <f t="shared" si="11"/>
-        <v>6.7338361550000059</v>
+        <v>5.2646478736999711</v>
       </c>
       <c r="M82">
         <v>3</v>
@@ -3024,7 +3028,7 @@
       </c>
       <c r="H83">
         <f t="shared" si="11"/>
-        <v>6.7320885029999999</v>
+        <v>5.266395525699977</v>
       </c>
       <c r="M83">
         <v>4</v>
@@ -3074,7 +3078,7 @@
       </c>
       <c r="H84">
         <f t="shared" si="11"/>
-        <v>7.5402330469999868</v>
+        <v>4.4582509816999902</v>
       </c>
       <c r="M84">
         <v>5</v>
@@ -3156,7 +3160,7 @@
       </c>
       <c r="H87">
         <f>ABS(E87-($K$87*1000))</f>
-        <v>10.766340587999991</v>
+        <v>1.232143440700014</v>
       </c>
       <c r="I87">
         <v>12.42</v>
@@ -3165,7 +3169,8 @@
         <v>-20.98</v>
       </c>
       <c r="K87" s="2">
-        <v>0.2</v>
+        <f>0.2+0.0119984840287</f>
+        <v>0.2119984840287</v>
       </c>
     </row>
     <row r="88" spans="2:19">
@@ -3191,7 +3196,7 @@
       </c>
       <c r="H88">
         <f t="shared" ref="H88:H91" si="14">ABS(E88-($K$87*1000))</f>
-        <v>10.566406276000009</v>
+        <v>1.4320777526999962</v>
       </c>
     </row>
     <row r="89" spans="2:19">
@@ -3217,7 +3222,7 @@
       </c>
       <c r="H89">
         <f t="shared" si="14"/>
-        <v>10.765881304999994</v>
+        <v>1.2326027237000119</v>
       </c>
     </row>
     <row r="90" spans="2:19">
@@ -3243,7 +3248,7 @@
       </c>
       <c r="H90">
         <f t="shared" si="14"/>
-        <v>10.566548366000006</v>
+        <v>1.4319356626999991</v>
       </c>
     </row>
     <row r="91" spans="2:19">
@@ -3269,7 +3274,7 @@
       </c>
       <c r="H91">
         <f t="shared" si="14"/>
-        <v>10.749504007000013</v>
+        <v>1.2489800216999924</v>
       </c>
     </row>
     <row r="93" spans="2:19">
@@ -3327,7 +3332,7 @@
       </c>
       <c r="H94">
         <f>ABS(E94-($K$94*1000))</f>
-        <v>7.4816371649999667</v>
+        <v>4.5168468637000387</v>
       </c>
       <c r="I94">
         <v>12.52</v>
@@ -3337,8 +3342,8 @@
         <v>29.48</v>
       </c>
       <c r="K94" s="2">
-        <f>0.4-0.209+0.003</f>
-        <v>0.19400000000000003</v>
+        <f>0.4-0.209+0.003+0.0119984840287</f>
+        <v>0.20599848402870002</v>
       </c>
     </row>
     <row r="95" spans="2:19">
@@ -3364,7 +3369,7 @@
       </c>
       <c r="H95">
         <f t="shared" ref="H95:H98" si="17">ABS(E95-($K$94*1000))</f>
-        <v>9.0053881299999716</v>
+        <v>2.9930958987000338</v>
       </c>
     </row>
     <row r="96" spans="2:19">
@@ -3390,7 +3395,7 @@
       </c>
       <c r="H96">
         <f t="shared" si="17"/>
-        <v>8.620646733999962</v>
+        <v>3.3778372947000435</v>
       </c>
     </row>
     <row r="97" spans="2:11">
@@ -3416,7 +3421,7 @@
       </c>
       <c r="H97">
         <f t="shared" si="17"/>
-        <v>9.002947598999981</v>
+        <v>2.9955364297000244</v>
       </c>
     </row>
     <row r="98" spans="2:11">
@@ -3442,7 +3447,7 @@
       </c>
       <c r="H98">
         <f t="shared" si="17"/>
-        <v>9.195186633999981</v>
+        <v>2.8032973947000244</v>
       </c>
     </row>
     <row r="100" spans="2:11">
@@ -3500,7 +3505,7 @@
       </c>
       <c r="H101">
         <f>ABS(E101-($K$101*1000))</f>
-        <v>8.4252686149999647</v>
+        <v>3.5732154137000407</v>
       </c>
       <c r="I101">
         <v>-13.65</v>
@@ -3510,8 +3515,8 @@
         <v>28.009999999999998</v>
       </c>
       <c r="K101" s="2">
-        <f>0.4-0.211+0.003</f>
-        <v>0.19200000000000003</v>
+        <f>0.4-0.211+0.003+0.0119984840287</f>
+        <v>0.20399848402870002</v>
       </c>
     </row>
     <row r="102" spans="2:11">
@@ -3537,7 +3542,7 @@
       </c>
       <c r="H102">
         <f t="shared" ref="H102:H105" si="20">ABS(E102-($K$101*1000))</f>
-        <v>8.4260584279999762</v>
+        <v>3.5724256007000292</v>
       </c>
     </row>
     <row r="103" spans="2:11">
@@ -3563,7 +3568,7 @@
       </c>
       <c r="H103">
         <f t="shared" si="20"/>
-        <v>8.420389178999983</v>
+        <v>3.5780948497000225</v>
       </c>
     </row>
     <row r="104" spans="2:11">
@@ -3589,7 +3594,7 @@
       </c>
       <c r="H104">
         <f t="shared" si="20"/>
-        <v>8.2330235279999613</v>
+        <v>3.7654605007000441</v>
       </c>
     </row>
     <row r="105" spans="2:11">
@@ -3615,7 +3620,7 @@
       </c>
       <c r="H105">
         <f t="shared" si="20"/>
-        <v>8.2009891909999624</v>
+        <v>3.797494837700043</v>
       </c>
     </row>
     <row r="107" spans="2:11">
@@ -3673,7 +3678,7 @@
       </c>
       <c r="H108">
         <f>ABS(E108-($K$108*1000))</f>
-        <v>14.599971224999962</v>
+        <v>2.6014871962999564</v>
       </c>
       <c r="I108">
         <v>-12.02</v>
@@ -3682,8 +3687,8 @@
         <v>-24.77</v>
       </c>
       <c r="K108" s="2">
-        <f>0.4-0.207+0.003</f>
-        <v>0.19600000000000004</v>
+        <f>0.4-0.207+0.003+0.0119984840287</f>
+        <v>0.20799848402870003</v>
       </c>
     </row>
     <row r="109" spans="2:11">
@@ -3709,7 +3714,7 @@
       </c>
       <c r="H109">
         <f t="shared" ref="H109:H112" si="23">ABS(E109-($K$108*1000))</f>
-        <v>14.600494568999977</v>
+        <v>2.6020105402999718</v>
       </c>
     </row>
     <row r="110" spans="2:11">
@@ -3735,7 +3740,7 @@
       </c>
       <c r="H110">
         <f t="shared" si="23"/>
-        <v>14.341732202999964</v>
+        <v>2.3432481742999585</v>
       </c>
     </row>
     <row r="111" spans="2:11">
@@ -3761,7 +3766,7 @@
       </c>
       <c r="H111">
         <f t="shared" si="23"/>
-        <v>14.539018256999981</v>
+        <v>2.5405342282999754</v>
       </c>
     </row>
     <row r="112" spans="2:11">
@@ -3787,7 +3792,7 @@
       </c>
       <c r="H112">
         <f t="shared" si="23"/>
-        <v>14.538928840999972</v>
+        <v>2.5404448122999668</v>
       </c>
     </row>
   </sheetData>
@@ -3810,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:T14"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3903,7 +3908,7 @@
       </c>
       <c r="H3">
         <f>ABS(E3-($K$3*1000))</f>
-        <v>8.9262729239999885</v>
+        <v>3.0722111047000169</v>
       </c>
       <c r="I3">
         <v>1.59</v>
@@ -3912,8 +3917,8 @@
         <v>3.61</v>
       </c>
       <c r="K3" s="2">
-        <f>0.4-0.201+0.003</f>
-        <v>0.20200000000000001</v>
+        <f>0.4-0.201+0.003+0.0119984840287</f>
+        <v>0.2139984840287</v>
       </c>
       <c r="O3">
         <f>AVERAGE(F3:F7,F10:F14,F17:F21,F24:F28)</f>
@@ -3933,11 +3938,11 @@
       </c>
       <c r="S3">
         <f>AVERAGE(H3:H7,H10:H14,H17:H21,H24:H28)</f>
-        <v>10.902600245649992</v>
+        <v>2.3394612909499926</v>
       </c>
       <c r="T3">
         <f>_xlfn.STDEV.P(H3:H7,H10:H14,H17:H21,H24:H28)</f>
-        <v>2.4367280742217923</v>
+        <v>1.2905525335294337</v>
       </c>
     </row>
     <row r="4" spans="2:20">
@@ -3963,7 +3968,7 @@
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H7" si="2">ABS(E4-($K$3*1000))</f>
-        <v>8.9141868950000003</v>
+        <v>3.0842971337000051</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>26</v>
@@ -3997,7 +4002,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>9.9707536390000087</v>
+        <v>2.0277303896999967</v>
       </c>
       <c r="O5" t="s">
         <v>21</v>
@@ -4041,7 +4046,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>9.1532804690000091</v>
+        <v>2.8452035596999963</v>
       </c>
       <c r="O6">
         <f>AVERAGE(F31:F35,F38:F42,F45:F49,F52:F56)</f>
@@ -4061,11 +4066,11 @@
       </c>
       <c r="S6">
         <f>AVERAGE(H31:H35,H38:H42,H45:H49,H52:H56)</f>
-        <v>11.945007182999978</v>
+        <v>1.6025620354100241</v>
       </c>
       <c r="T6">
         <f>_xlfn.STDEV.P(H31:H35,H38:H42,H45:H49,H52:H561)</f>
-        <v>3.2076058791807376</v>
+        <v>2.2193070676137543</v>
       </c>
     </row>
     <row r="7" spans="2:20">
@@ -4091,7 +4096,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>9.14050748599999</v>
+        <v>2.8579765427000154</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>24</v>
@@ -4171,11 +4176,11 @@
       </c>
       <c r="S9">
         <f>AVERAGE(H59:H63,H66:H70,H73:H77,H80:H84)</f>
-        <v>16.324651741849969</v>
+        <v>4.3849408243599983</v>
       </c>
       <c r="T9">
         <f>_xlfn.STDEV.P(H59:H63,H66:H70,H73:H77,H80:H84)</f>
-        <v>2.5622960703749942</v>
+        <v>2.4603622093955124</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -4201,7 +4206,7 @@
       </c>
       <c r="H10">
         <f>ABS(E10-($K$10*1000))</f>
-        <v>7.9811777810000137</v>
+        <v>4.0173062476999917</v>
       </c>
       <c r="I10">
         <v>3.07</v>
@@ -4210,8 +4215,8 @@
         <v>-3.91</v>
       </c>
       <c r="K10" s="2">
-        <f>0.4-0.201+0.003</f>
-        <v>0.20200000000000001</v>
+        <f>0.4-0.201+0.003+0.0119984840287</f>
+        <v>0.2139984840287</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>25</v>
@@ -4245,7 +4250,7 @@
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H14" si="5">ABS(E11-($K$10*1000))</f>
-        <v>8.0155520380000098</v>
+        <v>3.9829319906999956</v>
       </c>
       <c r="O11" t="s">
         <v>21</v>
@@ -4289,7 +4294,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="5"/>
-        <v>8.0104499569999916</v>
+        <v>3.9880340717000138</v>
       </c>
       <c r="O12">
         <f>AVERAGE(F87:F91,F94:F98,F101:F105,F108:F112)</f>
@@ -4309,11 +4314,11 @@
       </c>
       <c r="S12">
         <f>AVERAGE(H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>13.916532623499972</v>
+        <v>3.3181921509000007</v>
       </c>
       <c r="T12">
         <f>_xlfn.STDEV.P(H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>3.3360145491041271</v>
+        <v>1.9487186388892102</v>
       </c>
     </row>
     <row r="13" spans="2:20">
@@ -4339,7 +4344,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
-        <v>7.7679988479999906</v>
+        <v>4.2304851807000148</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>28</v>
@@ -4373,7 +4378,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="5"/>
-        <v>7.7512095099999954</v>
+        <v>4.24727451870001</v>
       </c>
       <c r="O14">
         <f>AVERAGE(F3:F7,F10:F14,F17:F21,F24:F28,F31:F35,F38:F42,F45:F49,F52:F56,F59:F63,F66:F70,F73:F77,F80:F84,F87:F91,F94:F98,F101:F105,F108:F112)</f>
@@ -4393,11 +4398,11 @@
       </c>
       <c r="S14">
         <f>AVERAGE(H3:H7,H10:H14,H17:H21,H24:H28,H31:H35,H38:H42,H45:H49,H52:H56,H59:H63,H66:H70,H73:H77,H80:H84,H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>13.272197948499979</v>
+        <v>2.911289075405004</v>
       </c>
       <c r="T14">
         <f>_xlfn.STDEV.P(H3:H7,H10:H14,H17:H21,H24:H28,H31:H35,H38:H42,H45:H49,H52:H56,H59:H63,H66:H70,H73:H77,H80:H84,H87:H91,H94:H98,H101:H105,H108:H112)</f>
-        <v>3.3275557032891112</v>
+        <v>2.0541105197655893</v>
       </c>
     </row>
     <row r="16" spans="2:20">
@@ -4455,7 +4460,7 @@
       </c>
       <c r="H17">
         <f>ABS(E17-($K$17*1000))</f>
-        <v>12.501748937999963</v>
+        <v>0.50326490929995771</v>
       </c>
       <c r="I17">
         <v>2.16</v>
@@ -4464,8 +4469,8 @@
         <v>0.93</v>
       </c>
       <c r="K17" s="2">
-        <f>0.4-0.209+0.003</f>
-        <v>0.19400000000000003</v>
+        <f>0.4-0.209+0.003+0.0119984840287</f>
+        <v>0.20599848402870002</v>
       </c>
     </row>
     <row r="18" spans="2:22">
@@ -4491,7 +4496,7 @@
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H21" si="8">ABS(E18-($K$17*1000))</f>
-        <v>12.695835225999986</v>
+        <v>0.69735119729998019</v>
       </c>
     </row>
     <row r="19" spans="2:22">
@@ -4517,7 +4522,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="8"/>
-        <v>12.68130907699998</v>
+        <v>0.68282504829997492</v>
       </c>
     </row>
     <row r="20" spans="2:22">
@@ -4543,7 +4548,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="8"/>
-        <v>12.470846523999967</v>
+        <v>0.47236249529996144</v>
       </c>
     </row>
     <row r="21" spans="2:22">
@@ -4569,7 +4574,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="8"/>
-        <v>12.68286754899998</v>
+        <v>0.68438352029997418</v>
       </c>
     </row>
     <row r="23" spans="2:22">
@@ -4657,7 +4662,7 @@
       </c>
       <c r="H24">
         <f>ABS(E24-($K$24*1000))</f>
-        <v>13.79018074199999</v>
+        <v>1.7916967132999844</v>
       </c>
       <c r="I24">
         <v>-2.1</v>
@@ -4666,7 +4671,8 @@
         <v>-4.62</v>
       </c>
       <c r="K24" s="2">
-        <v>0.19500000000000001</v>
+        <f>0.195+0.0119984840287</f>
+        <v>0.2069984840287</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -4690,7 +4696,7 @@
       </c>
       <c r="S24">
         <f>ABS(P24-($V$24*1000))</f>
-        <v>11.471730990999959</v>
+        <v>0.52675303770004689</v>
       </c>
       <c r="T24">
         <v>-2.0499999999999998</v>
@@ -4699,8 +4705,8 @@
         <v>0.24</v>
       </c>
       <c r="V24" s="2">
-        <f>0.4-0.207+0.003</f>
-        <v>0.19600000000000004</v>
+        <f>0.4-0.207+0.003+0.0119984840287</f>
+        <v>0.20799848402870003</v>
       </c>
     </row>
     <row r="25" spans="2:22">
@@ -4726,7 +4732,7 @@
       </c>
       <c r="H25">
         <f>ABS(E25-($K$24*1000))</f>
-        <v>13.998223591999988</v>
+        <v>1.9997395632999826</v>
       </c>
       <c r="M25">
         <v>2</v>
@@ -4750,7 +4756,7 @@
       </c>
       <c r="S25">
         <f>ABS(P25-($V$24*1000))</f>
-        <v>12.05622075399998</v>
+        <v>5.7736725299974978E-2</v>
       </c>
     </row>
     <row r="26" spans="2:22">
@@ -4776,7 +4782,7 @@
       </c>
       <c r="H26">
         <f>ABS(E26-($K$24*1000))</f>
-        <v>13.795516980000002</v>
+        <v>1.7970329512999967</v>
       </c>
       <c r="M26">
         <v>3</v>
@@ -4800,7 +4806,7 @@
       </c>
       <c r="S26">
         <f>ABS(P26-($V$24*1000))</f>
-        <v>12.047191220999963</v>
+        <v>4.8707192299957569E-2</v>
       </c>
     </row>
     <row r="27" spans="2:22">
@@ -4826,7 +4832,7 @@
       </c>
       <c r="H27">
         <f>ABS(E27-($K$24*1000))</f>
-        <v>14.001283059000002</v>
+        <v>2.0027990302999967</v>
       </c>
       <c r="M27">
         <v>4</v>
@@ -4850,7 +4856,7 @@
       </c>
       <c r="S27">
         <f>ABS(P27-($V$24*1000))</f>
-        <v>12.055601672999984</v>
+        <v>5.7117644299978565E-2</v>
       </c>
     </row>
     <row r="28" spans="2:22">
@@ -4876,7 +4882,7 @@
       </c>
       <c r="H28">
         <f>ABS(E28-($K$24*1000))</f>
-        <v>13.802803678999993</v>
+        <v>1.8043196502999876</v>
       </c>
       <c r="M28">
         <v>5</v>
@@ -4900,7 +4906,7 @@
       </c>
       <c r="S28">
         <f>ABS(P28-($V$24*1000))</f>
-        <v>12.245287199999979</v>
+        <v>0.2468031712999732</v>
       </c>
     </row>
     <row r="30" spans="2:22">
@@ -4958,7 +4964,7 @@
       </c>
       <c r="H31">
         <f>ABS(E31-($K$31*1000))</f>
-        <v>10.631084297999962</v>
+        <v>1.3673997307000434</v>
       </c>
       <c r="I31">
         <v>-6.32</v>
@@ -4967,8 +4973,8 @@
         <v>3.74</v>
       </c>
       <c r="K31">
-        <f>0.4-0.208+0.003</f>
-        <v>0.19500000000000003</v>
+        <f>0.4-0.208+0.003+0.0119984840287</f>
+        <v>0.20699848402870002</v>
       </c>
     </row>
     <row r="32" spans="2:22">
@@ -4994,7 +5000,7 @@
       </c>
       <c r="H32">
         <f>ABS(E32-($K$31*1000))</f>
-        <v>10.63091805199997</v>
+        <v>1.3675659767000354</v>
       </c>
     </row>
     <row r="33" spans="2:11">
@@ -5020,7 +5026,7 @@
       </c>
       <c r="H33">
         <f>ABS(E33-($K$31*1000))</f>
-        <v>10.634192189999965</v>
+        <v>1.3642918387000407</v>
       </c>
     </row>
     <row r="34" spans="2:11">
@@ -5046,7 +5052,7 @@
       </c>
       <c r="H34">
         <f>ABS(E34-($K$31*1000))</f>
-        <v>10.628538014999975</v>
+        <v>1.3699460137000301</v>
       </c>
     </row>
     <row r="35" spans="2:11">
@@ -5072,7 +5078,7 @@
       </c>
       <c r="H35">
         <f>ABS(E35-($K$31*1000))</f>
-        <v>11.597996188999986</v>
+        <v>0.40048783970001978</v>
       </c>
     </row>
     <row r="37" spans="2:11">
@@ -5130,7 +5136,7 @@
       </c>
       <c r="H38">
         <f>ABS(E38-($K$38*1000))</f>
-        <v>12.310219405999959</v>
+        <v>0.3117353772999536</v>
       </c>
       <c r="I38">
         <v>-5.48</v>
@@ -5139,8 +5145,8 @@
         <v>-4.83</v>
       </c>
       <c r="K38" s="2">
-        <f>0.4-0.208+0.003</f>
-        <v>0.19500000000000003</v>
+        <f>0.4-0.208+0.003+0.0119984840287</f>
+        <v>0.20699848402870002</v>
       </c>
     </row>
     <row r="39" spans="2:11">
@@ -5166,7 +5172,7 @@
       </c>
       <c r="H39">
         <f>ABS(E39-($K$38*1000))</f>
-        <v>12.12928438199998</v>
+        <v>0.13080035329997486</v>
       </c>
     </row>
     <row r="40" spans="2:11">
@@ -5192,7 +5198,7 @@
       </c>
       <c r="H40">
         <f>ABS(E40-($K$38*1000))</f>
-        <v>11.528884818999984</v>
+        <v>0.46959920970002145</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -5218,7 +5224,7 @@
       </c>
       <c r="H41">
         <f>ABS(E41-($K$38*1000))</f>
-        <v>11.53599567599997</v>
+        <v>0.46248835270003497</v>
       </c>
     </row>
     <row r="42" spans="2:11">
@@ -5244,7 +5250,7 @@
       </c>
       <c r="H42">
         <f>ABS(E42-($K$38*1000))</f>
-        <v>11.534662727999972</v>
+        <v>0.46382130070003313</v>
       </c>
     </row>
     <row r="44" spans="2:11">
@@ -5302,7 +5308,7 @@
       </c>
       <c r="H45">
         <f>ABS(E45-($K$45*1000))</f>
-        <v>10.01537292499998</v>
+        <v>1.9831111037000255</v>
       </c>
       <c r="I45">
         <v>-5.32</v>
@@ -5311,8 +5317,8 @@
         <v>0.87</v>
       </c>
       <c r="K45" s="2">
-        <f>0.4-0.208+0.003</f>
-        <v>0.19500000000000003</v>
+        <f>0.4-0.208+0.003+0.0119984840287</f>
+        <v>0.20699848402870002</v>
       </c>
     </row>
     <row r="46" spans="2:11">
@@ -5338,7 +5344,7 @@
       </c>
       <c r="H46">
         <f>ABS(E46-($K$45*1000))</f>
-        <v>10.231430974999967</v>
+        <v>1.7670530537000388</v>
       </c>
     </row>
     <row r="47" spans="2:11">
@@ -5364,7 +5370,7 @@
       </c>
       <c r="H47">
         <f>ABS(E47-($K$45*1000))</f>
-        <v>10.229223103999971</v>
+        <v>1.7692609247000348</v>
       </c>
     </row>
     <row r="48" spans="2:11">
@@ -5390,7 +5396,7 @@
       </c>
       <c r="H48">
         <f>ABS(E48-($K$45*1000))</f>
-        <v>10.197078377999958</v>
+        <v>1.8014056507000475</v>
       </c>
     </row>
     <row r="49" spans="2:11">
@@ -5416,7 +5422,7 @@
       </c>
       <c r="H49">
         <f>ABS(E49-($K$45*1000))</f>
-        <v>10.024526212999973</v>
+        <v>1.9739578157000324</v>
       </c>
     </row>
     <row r="51" spans="2:11">
@@ -5474,7 +5480,7 @@
       </c>
       <c r="H52">
         <f>ABS(E52-($K$52*1000))</f>
-        <v>15.040988363999986</v>
+        <v>3.0425043353000092</v>
       </c>
       <c r="I52">
         <v>-4.63</v>
@@ -5483,7 +5489,8 @@
         <v>6.75</v>
       </c>
       <c r="K52" s="2">
-        <v>0.186</v>
+        <f>0.186+0.0119984840287</f>
+        <v>0.19799848402869999</v>
       </c>
     </row>
     <row r="53" spans="2:11">
@@ -5509,7 +5516,7 @@
       </c>
       <c r="H53">
         <f>ABS(E53-($K$52*1000))</f>
-        <v>15.039912914000013</v>
+        <v>3.0414288853000357</v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -5535,7 +5542,7 @@
       </c>
       <c r="H54">
         <f>ABS(E54-($K$52*1000))</f>
-        <v>14.863325975999999</v>
+        <v>2.8648419473000217</v>
       </c>
     </row>
     <row r="55" spans="2:11">
@@ -5561,7 +5568,7 @@
       </c>
       <c r="H55">
         <f>ABS(E55-($K$52*1000))</f>
-        <v>15.047766612000004</v>
+        <v>3.0492825833000268</v>
       </c>
     </row>
     <row r="56" spans="2:11">
@@ -5587,7 +5594,7 @@
       </c>
       <c r="H56">
         <f>ABS(E56-($K$52*1000))</f>
-        <v>15.048742443999998</v>
+        <v>3.0502584153000214</v>
       </c>
     </row>
     <row r="58" spans="2:11">
@@ -5645,7 +5652,7 @@
       </c>
       <c r="H59">
         <f>ABS(E59-($K$59*1000))</f>
-        <v>12.126861804999976</v>
+        <v>0.12837777629999891</v>
       </c>
       <c r="I59">
         <v>7.03</v>
@@ -5654,8 +5661,8 @@
         <v>10.84</v>
       </c>
       <c r="K59" s="2">
-        <f>0.4-0.215+0.003</f>
-        <v>0.18800000000000003</v>
+        <f>0.4-0.215+0.003+0.0119984840287</f>
+        <v>0.19999848402870002</v>
       </c>
     </row>
     <row r="60" spans="2:11">
@@ -5681,7 +5688,7 @@
       </c>
       <c r="H60">
         <f>ABS(E60-($K$59*1000))</f>
-        <v>11.944644709999977</v>
+        <v>5.3839318699999694E-2</v>
       </c>
     </row>
     <row r="61" spans="2:11">
@@ -5707,7 +5714,7 @@
       </c>
       <c r="H61">
         <f>ABS(E61-($K$59*1000))</f>
-        <v>11.731559889999971</v>
+        <v>0.26692413870000564</v>
       </c>
     </row>
     <row r="62" spans="2:11">
@@ -5733,7 +5740,7 @@
       </c>
       <c r="H62">
         <f>ABS(E62-($K$59*1000))</f>
-        <v>12.266358056999962</v>
+        <v>0.26787402829998541</v>
       </c>
     </row>
     <row r="63" spans="2:11">
@@ -5759,7 +5766,7 @@
       </c>
       <c r="H63">
         <f>ABS(E63-($K$59*1000))</f>
-        <v>11.731516373999966</v>
+        <v>0.26696765470001083</v>
       </c>
     </row>
     <row r="65" spans="2:22">
@@ -5817,7 +5824,7 @@
       </c>
       <c r="H66">
         <f>ABS(E66-($K$66*1000))</f>
-        <v>17.819315561999986</v>
+        <v>5.8208315333000087</v>
       </c>
       <c r="I66">
         <v>-8.6300000000000008</v>
@@ -5826,8 +5833,8 @@
         <v>10.59</v>
       </c>
       <c r="K66" s="2">
-        <f>0.4-0.224+0.003</f>
-        <v>0.17900000000000002</v>
+        <f>0.4-0.224+0.003+0.0119984840287</f>
+        <v>0.19099848402870001</v>
       </c>
     </row>
     <row r="67" spans="2:22">
@@ -5853,7 +5860,7 @@
       </c>
       <c r="H67">
         <f>ABS(E67-($K$66*1000))</f>
-        <v>17.803192785999983</v>
+        <v>5.8047087573000056</v>
       </c>
     </row>
     <row r="68" spans="2:22">
@@ -5879,7 +5886,7 @@
       </c>
       <c r="H68">
         <f>ABS(E68-($K$66*1000))</f>
-        <v>17.79606087999997</v>
+        <v>5.7975768512999935</v>
       </c>
     </row>
     <row r="69" spans="2:22">
@@ -5905,7 +5912,7 @@
       </c>
       <c r="H69">
         <f>ABS(E69-($K$66*1000))</f>
-        <v>16.927299685999969</v>
+        <v>4.9288156572999924</v>
       </c>
     </row>
     <row r="70" spans="2:22">
@@ -5931,7 +5938,7 @@
       </c>
       <c r="H70">
         <f>ABS(E70-($K$66*1000))</f>
-        <v>17.269592029999984</v>
+        <v>5.2711080013000071</v>
       </c>
     </row>
     <row r="72" spans="2:22">
@@ -5990,7 +5997,7 @@
       </c>
       <c r="H73">
         <f>ABS(E73-($K$73*1000))</f>
-        <v>17.380369983999969</v>
+        <v>5.3818859552999925</v>
       </c>
       <c r="I73">
         <v>-7.91</v>
@@ -5999,8 +6006,8 @@
         <v>-9.6300000000000008</v>
       </c>
       <c r="K73" s="2">
-        <f>0.4-0.22+0.003</f>
-        <v>0.18300000000000002</v>
+        <f>0.4-0.22+0.003+0.0119984840287</f>
+        <v>0.19499848402870001</v>
       </c>
       <c r="V73" s="2"/>
     </row>
@@ -6027,7 +6034,7 @@
       </c>
       <c r="H74">
         <f>ABS(E74-($K$73*1000))</f>
-        <v>17.380558816999979</v>
+        <v>5.3820747883000024</v>
       </c>
     </row>
     <row r="75" spans="2:22">
@@ -6053,7 +6060,7 @@
       </c>
       <c r="H75">
         <f>ABS(E75-($K$73*1000))</f>
-        <v>17.379493273999969</v>
+        <v>5.3810092452999925</v>
       </c>
     </row>
     <row r="76" spans="2:22">
@@ -6079,7 +6086,7 @@
       </c>
       <c r="H76">
         <f>ABS(E76-($K$73*1000))</f>
-        <v>17.36833926099996</v>
+        <v>5.3698552322999831</v>
       </c>
     </row>
     <row r="77" spans="2:22">
@@ -6105,7 +6112,7 @@
       </c>
       <c r="H77">
         <f>ABS(E77-($K$73*1000))</f>
-        <v>17.367671573999985</v>
+        <v>5.369187545300008</v>
       </c>
     </row>
     <row r="79" spans="2:22">
@@ -6164,7 +6171,7 @@
       </c>
       <c r="H80">
         <f>ABS(E80-($K$80*1000))</f>
-        <v>18.517563912999975</v>
+        <v>6.5190798842999982</v>
       </c>
       <c r="I80">
         <v>12.51</v>
@@ -6173,8 +6180,8 @@
         <v>-8.7899999999999991</v>
       </c>
       <c r="K80" s="2">
-        <f>0.4-0.217+0.003</f>
-        <v>0.18600000000000003</v>
+        <f>0.4-0.217+0.003+0.0119984840287</f>
+        <v>0.19799848402870002</v>
       </c>
       <c r="V80" s="2"/>
     </row>
@@ -6201,7 +6208,7 @@
       </c>
       <c r="H81">
         <f>ABS(E81-($K$80*1000))</f>
-        <v>18.688604559999959</v>
+        <v>6.6901205312999821</v>
       </c>
     </row>
     <row r="82" spans="2:11">
@@ -6227,7 +6234,7 @@
       </c>
       <c r="H82">
         <f>ABS(E82-($K$80*1000))</f>
-        <v>18.329063758999979</v>
+        <v>6.330579730300002</v>
       </c>
     </row>
     <row r="83" spans="2:11">
@@ -6253,7 +6260,7 @@
       </c>
       <c r="H83">
         <f>ABS(E83-($K$80*1000))</f>
-        <v>18.335034053999976</v>
+        <v>6.3365500252999993</v>
       </c>
     </row>
     <row r="84" spans="2:11">
@@ -6279,7 +6286,7 @@
       </c>
       <c r="H84">
         <f>ABS(E84-($K$80*1000))</f>
-        <v>18.329933860999972</v>
+        <v>6.3314498322999953</v>
       </c>
     </row>
     <row r="86" spans="2:11">
@@ -6337,7 +6344,7 @@
       </c>
       <c r="H87">
         <f>ABS(E87-($K$87*1000))</f>
-        <v>17.15044577599997</v>
+        <v>5.1519617472999926</v>
       </c>
       <c r="I87">
         <v>19.36</v>
@@ -6346,8 +6353,8 @@
         <v>-20.93</v>
       </c>
       <c r="K87" s="2">
-        <f>0.4-0.215+0.003</f>
-        <v>0.18800000000000003</v>
+        <f>0.4-0.215+0.003+0.0119984840287</f>
+        <v>0.19999848402870002</v>
       </c>
     </row>
     <row r="88" spans="2:11">
@@ -6373,7 +6380,7 @@
       </c>
       <c r="H88">
         <f>ABS(E88-($K$87*1000))</f>
-        <v>17.15057825599996</v>
+        <v>5.1520942272999832</v>
       </c>
     </row>
     <row r="89" spans="2:11">
@@ -6399,7 +6406,7 @@
       </c>
       <c r="H89">
         <f>ABS(E89-($K$87*1000))</f>
-        <v>17.344598650999984</v>
+        <v>5.3461146223000071</v>
       </c>
     </row>
     <row r="90" spans="2:11">
@@ -6425,7 +6432,7 @@
       </c>
       <c r="H90">
         <f>ABS(E90-($K$87*1000))</f>
-        <v>17.152111080999958</v>
+        <v>5.1536270522999814</v>
       </c>
     </row>
     <row r="91" spans="2:11">
@@ -6451,7 +6458,7 @@
       </c>
       <c r="H91">
         <f>ABS(E91-($K$87*1000))</f>
-        <v>17.150580798999982</v>
+        <v>5.1520967703000053</v>
       </c>
     </row>
     <row r="93" spans="2:11">
@@ -6509,7 +6516,7 @@
       </c>
       <c r="H94">
         <f>ABS(E94-($K$94*1000))</f>
-        <v>11.235129822999966</v>
+        <v>0.76335420570003976</v>
       </c>
       <c r="I94">
         <v>17.399999999999999</v>
@@ -6518,8 +6525,8 @@
         <v>20.98</v>
       </c>
       <c r="K94" s="2">
-        <f>0.4-0.208+0.003</f>
-        <v>0.19500000000000003</v>
+        <f>0.4-0.208+0.003+0.0119984840287</f>
+        <v>0.20699848402870002</v>
       </c>
     </row>
     <row r="95" spans="2:11">
@@ -6545,7 +6552,7 @@
       </c>
       <c r="H95">
         <f>ABS(E95-($K$94*1000))</f>
-        <v>10.413163249999968</v>
+        <v>1.5853207787000372</v>
       </c>
     </row>
     <row r="96" spans="2:11">
@@ -6571,7 +6578,7 @@
       </c>
       <c r="H96">
         <f>ABS(E96-($K$94*1000))</f>
-        <v>11.000075397999979</v>
+        <v>0.99840863070002683</v>
       </c>
     </row>
     <row r="97" spans="2:11">
@@ -6597,7 +6604,7 @@
       </c>
       <c r="H97">
         <f>ABS(E97-($K$94*1000))</f>
-        <v>11.184506556999963</v>
+        <v>0.81397747170004209</v>
       </c>
     </row>
     <row r="98" spans="2:11">
@@ -6623,7 +6630,7 @@
       </c>
       <c r="H98">
         <f>ABS(E98-($K$94*1000))</f>
-        <v>11.011070572999984</v>
+        <v>0.98741345570002181</v>
       </c>
     </row>
     <row r="100" spans="2:11">
@@ -6681,7 +6688,7 @@
       </c>
       <c r="H101">
         <f>ABS(E101-($K$101*1000))</f>
-        <v>10.498410277999966</v>
+        <v>1.500073750700011</v>
       </c>
       <c r="I101">
         <v>-19.98</v>
@@ -6690,8 +6697,8 @@
         <v>20.79</v>
       </c>
       <c r="K101" s="2">
-        <f>0.4-0.215+0.003</f>
-        <v>0.18800000000000003</v>
+        <f>0.4-0.215+0.003+0.0119984840287</f>
+        <v>0.19999848402870002</v>
       </c>
     </row>
     <row r="102" spans="2:11">
@@ -6717,7 +6724,7 @@
       </c>
       <c r="H102">
         <f>ABS(E102-($K$101*1000))</f>
-        <v>10.110383355999971</v>
+        <v>1.8881006727000056</v>
       </c>
     </row>
     <row r="103" spans="2:11">
@@ -6743,7 +6750,7 @@
       </c>
       <c r="H103">
         <f>ABS(E103-($K$101*1000))</f>
-        <v>10.310612895999981</v>
+        <v>1.6878711326999962</v>
       </c>
     </row>
     <row r="104" spans="2:11">
@@ -6769,7 +6776,7 @@
       </c>
       <c r="H104">
         <f>ABS(E104-($K$101*1000))</f>
-        <v>10.109532160999976</v>
+        <v>1.8889518677000012</v>
       </c>
     </row>
     <row r="105" spans="2:11">
@@ -6795,7 +6802,7 @@
       </c>
       <c r="H105">
         <f>ABS(E105-($K$101*1000))</f>
-        <v>10.110520433999966</v>
+        <v>1.8879635947000111</v>
       </c>
     </row>
     <row r="107" spans="2:11">
@@ -6853,7 +6860,7 @@
       </c>
       <c r="H108">
         <f>ABS(E108-($K$108*1000))</f>
-        <v>17.245509046999985</v>
+        <v>5.2470250182999791</v>
       </c>
       <c r="I108">
         <v>-21.72</v>
@@ -6862,8 +6869,8 @@
         <v>-20.03</v>
       </c>
       <c r="K108" s="2">
-        <f>0.4-0.214+0.003</f>
-        <v>0.18900000000000003</v>
+        <f>0.4-0.214+0.003+0.0119984840287</f>
+        <v>0.20099848402870002</v>
       </c>
     </row>
     <row r="109" spans="2:11">
@@ -6889,7 +6896,7 @@
       </c>
       <c r="H109">
         <f>ABS(E109-($K$108*1000))</f>
-        <v>17.048120671999982</v>
+        <v>5.0496366432999764</v>
       </c>
     </row>
     <row r="110" spans="2:11">
@@ -6915,7 +6922,7 @@
       </c>
       <c r="H110">
         <f>ABS(E110-($K$108*1000))</f>
-        <v>17.048115921999965</v>
+        <v>5.04963189329996</v>
       </c>
     </row>
     <row r="111" spans="2:11">
@@ -6941,7 +6948,7 @@
       </c>
       <c r="H111">
         <f>ABS(E111-($K$108*1000))</f>
-        <v>17.240199277999977</v>
+        <v>5.2417152492999719</v>
       </c>
     </row>
     <row r="112" spans="2:11">
@@ -6967,7 +6974,7 @@
       </c>
       <c r="H112">
         <f>ABS(E112-($K$108*1000))</f>
-        <v>17.816988261999967</v>
+        <v>5.8185042332999615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>